<commit_message>
Update resultat to change baseline
</commit_message>
<xml_diff>
--- a/resultat-A2.xlsx
+++ b/resultat-A2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wiill\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5264F0D-C0FF-49E6-8146-F6EDBF5AFBF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C075F41-6896-466B-863A-371C5731CA26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10650" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{D8849010-B00D-4BCE-B925-700849EE8AB8}"/>
+    <workbookView xWindow="13305" yWindow="3405" windowWidth="28770" windowHeight="16170" activeTab="1" xr2:uid="{D8849010-B00D-4BCE-B925-700849EE8AB8}"/>
   </bookViews>
   <sheets>
     <sheet name="HadoopVSLinux" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -171,11 +171,11 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2691,34 +2691,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1.0973333333333337</c:v>
+                  <c:v>0.98066666666666702</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.36433333333333318</c:v>
+                  <c:v>0.24766666666666648</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.42933333333333357</c:v>
+                  <c:v>0.31266666666666687</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.71400000000000086</c:v>
+                  <c:v>0.59733333333333416</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.1333333333333258E-2</c:v>
+                  <c:v>-3.5333333333333439E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.10133333333333372</c:v>
+                  <c:v>-1.5333333333332977E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.3660000000000001</c:v>
+                  <c:v>0.24933333333333341</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>-0.1166666666666667</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.1166666666666667</c:v>
-                </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.0623333333333336</c:v>
+                  <c:v>0.94566666666666688</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2798,34 +2798,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.41266666666666829</c:v>
+                  <c:v>0.15233333333333388</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.16300000000000026</c:v>
+                  <c:v>-9.733333333333416E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.4333333333334046E-2</c:v>
+                  <c:v>-0.16600000000000037</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.30000000000000071</c:v>
+                  <c:v>3.9666666666666295E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.18866666666666809</c:v>
+                  <c:v>-7.1666666666666323E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.30400000000000116</c:v>
+                  <c:v>4.3666666666666742E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.14000000000000057</c:v>
+                  <c:v>-0.12033333333333385</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>-0.26033333333333442</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.26033333333333442</c:v>
-                </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.97500000000000053</c:v>
+                  <c:v>0.71466666666666612</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3012,34 +3012,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.93666666666666387</c:v>
+                  <c:v>0.52633333333332999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.13733333333333064</c:v>
+                  <c:v>-0.27300000000000324</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.18066666666666364</c:v>
+                  <c:v>-0.22966666666667024</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.2456666666666649</c:v>
+                  <c:v>0.83533333333333104</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>-0.41033333333333388</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.46733333333333249</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.16866666666666319</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.16766666666666907</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.87766666666666637</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.57899999999999707</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.24266666666666481</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.41033333333333388</c:v>
-                </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.4706666666666628</c:v>
+                  <c:v>1.0603333333333289</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3226,34 +3226,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>4.3333333333333335E-2</c:v>
+                  <c:v>-1.0999999999999899E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.5999999999999974E-2</c:v>
+                  <c:v>4.1666666666666741E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.9333333333333211E-2</c:v>
+                  <c:v>-2.5000000000000022E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.8333333333333321E-2</c:v>
+                  <c:v>-2.5999999999999912E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.3999999999999901E-2</c:v>
+                  <c:v>-4.0333333333333332E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.1333333333333342E-2</c:v>
+                  <c:v>-2.9999999999998916E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.5666666666666633E-2</c:v>
+                  <c:v>-8.6666666666666003E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>-5.4333333333333234E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="8">
-                  <c:v>5.4333333333333234E-2</c:v>
-                </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.3666666666666631E-2</c:v>
+                  <c:v>-1.0666666666666602E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6097,8 +6097,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D57CDF8-2E49-435E-BE00-1018393827E8}">
   <dimension ref="A1:U28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="X35" sqref="X35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6107,16 +6107,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1" t="s">
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
       <c r="J1" cm="1">
         <f t="array" ref="J1:U7">TRANSPOSE(A1:G12)</f>
         <v>0</v>
@@ -6156,25 +6156,25 @@
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>22</v>
       </c>
       <c r="J2" t="str">
@@ -6814,16 +6814,16 @@
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1" t="s">
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
       <c r="J17">
         <v>0</v>
       </c>
@@ -6862,25 +6862,25 @@
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="E18" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="F18" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="G18" s="1" t="s">
         <v>22</v>
       </c>
       <c r="J18">
@@ -7227,8 +7227,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{239EBBCB-277D-4169-A2F4-C750912E9025}">
   <dimension ref="A1:AC32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:G2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="N39" sqref="N39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7236,34 +7236,35 @@
     <col min="1" max="1" width="28.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="28.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="15" width="12" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1" t="s">
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="J1" s="1" t="s">
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="J1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1" t="s">
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
       <c r="R1" cm="1">
         <f t="array" ref="R1:AC7">TRANSPOSE(I1:O12)</f>
         <v>0</v>
       </c>
-      <c r="S1" s="2" t="str">
+      <c r="S1" s="1" t="str">
         <v>dataset</v>
       </c>
       <c r="T1" t="str">
@@ -7298,52 +7299,52 @@
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="M2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="N2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="O2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="R2" s="3" t="str">
+      <c r="R2" s="2" t="str">
         <v>Hadoop</v>
       </c>
-      <c r="S2" s="2" t="str">
+      <c r="S2" s="1" t="str">
         <v>hadoop real</v>
       </c>
       <c r="T2">
@@ -7426,10 +7427,10 @@
         <f t="shared" si="0"/>
         <v>0.76866666666666672</v>
       </c>
-      <c r="R3" s="3">
+      <c r="R3" s="2">
         <v>0</v>
       </c>
-      <c r="S3" s="2" t="str">
+      <c r="S3" s="1" t="str">
         <v>hadoop user</v>
       </c>
       <c r="T3">
@@ -7512,10 +7513,10 @@
         <f t="shared" si="1"/>
         <v>0.82133333333333336</v>
       </c>
-      <c r="R4" s="3">
+      <c r="R4" s="2">
         <v>0</v>
       </c>
-      <c r="S4" s="2" t="str">
+      <c r="S4" s="1" t="str">
         <v>hadoop sys</v>
       </c>
       <c r="T4">
@@ -7598,10 +7599,10 @@
         <f t="shared" si="2"/>
         <v>0.7546666666666666</v>
       </c>
-      <c r="R5" s="3" t="str">
+      <c r="R5" s="2" t="str">
         <v>Spark</v>
       </c>
-      <c r="S5" s="2" t="str">
+      <c r="S5" s="1" t="str">
         <v>spark real</v>
       </c>
       <c r="T5">
@@ -7684,10 +7685,10 @@
         <f t="shared" si="3"/>
         <v>0.75366666666666671</v>
       </c>
-      <c r="R6" s="3">
+      <c r="R6" s="2">
         <v>0</v>
       </c>
-      <c r="S6" s="2" t="str">
+      <c r="S6" s="1" t="str">
         <v>spark user</v>
       </c>
       <c r="T6">
@@ -7770,10 +7771,10 @@
         <f t="shared" si="4"/>
         <v>0.73933333333333329</v>
       </c>
-      <c r="R7" s="3">
+      <c r="R7" s="2">
         <v>0</v>
       </c>
-      <c r="S7" s="2" t="str">
+      <c r="S7" s="1" t="str">
         <v>spark sys</v>
       </c>
       <c r="T7">
@@ -8162,16 +8163,16 @@
       <c r="G15">
         <v>0.69199999999999995</v>
       </c>
-      <c r="J15" s="1" t="s">
+      <c r="J15" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
-      <c r="M15" s="1" t="s">
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="N15" s="1"/>
-      <c r="O15" s="1"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
       <c r="R15" t="str">
         <v>Hadoop</v>
       </c>
@@ -8179,34 +8180,34 @@
         <v>hadoop real</v>
       </c>
       <c r="T15">
-        <v>1.0973333333333337</v>
+        <v>0.98066666666666702</v>
       </c>
       <c r="U15">
-        <v>0.36433333333333318</v>
+        <v>0.24766666666666648</v>
       </c>
       <c r="V15">
-        <v>0.42933333333333357</v>
+        <v>0.31266666666666687</v>
       </c>
       <c r="W15">
-        <v>0.71400000000000086</v>
+        <v>0.59733333333333416</v>
       </c>
       <c r="X15">
-        <v>8.1333333333333258E-2</v>
+        <v>-3.5333333333333439E-2</v>
       </c>
       <c r="Y15">
-        <v>0.10133333333333372</v>
+        <v>-1.5333333333332977E-2</v>
       </c>
       <c r="Z15">
-        <v>0.3660000000000001</v>
+        <v>0.24933333333333341</v>
       </c>
       <c r="AA15">
+        <v>-0.1166666666666667</v>
+      </c>
+      <c r="AB15">
         <v>0</v>
       </c>
-      <c r="AB15">
-        <v>0.1166666666666667</v>
-      </c>
       <c r="AC15">
-        <v>1.0623333333333336</v>
+        <v>0.94566666666666688</v>
       </c>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.25">
@@ -8231,25 +8232,25 @@
       <c r="G16">
         <v>0.72</v>
       </c>
-      <c r="I16" s="2" t="s">
+      <c r="I16" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="J16" s="2" t="s">
+      <c r="J16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K16" s="2" t="s">
+      <c r="K16" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L16" s="2" t="s">
+      <c r="L16" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="M16" s="2" t="s">
+      <c r="M16" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="N16" s="2" t="s">
+      <c r="N16" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="O16" s="2" t="s">
+      <c r="O16" s="1" t="s">
         <v>19</v>
       </c>
       <c r="R16">
@@ -8315,11 +8316,11 @@
         <v>1</v>
       </c>
       <c r="J17">
-        <f>AVERAGE(B$3:B$5)-MIN(J3:J12)</f>
-        <v>1.0973333333333337</v>
+        <f>AVERAGE(B$3:B$5)-J$11</f>
+        <v>0.98066666666666702</v>
       </c>
       <c r="K17">
-        <f t="shared" ref="K17:O17" si="10">AVERAGE(C$3:C$5)-MIN(K3:K12)</f>
+        <f t="shared" ref="K17:O17" si="10">AVERAGE(C$3:C$5)-K$11</f>
         <v>1.2506666666666684</v>
       </c>
       <c r="L17">
@@ -8328,15 +8329,15 @@
       </c>
       <c r="M17">
         <f t="shared" si="10"/>
-        <v>0.41266666666666829</v>
+        <v>0.15233333333333388</v>
       </c>
       <c r="N17">
         <f t="shared" si="10"/>
-        <v>0.93666666666666387</v>
+        <v>0.52633333333332999</v>
       </c>
       <c r="O17">
         <f t="shared" si="10"/>
-        <v>4.3333333333333335E-2</v>
+        <v>-1.0999999999999899E-2</v>
       </c>
       <c r="R17">
         <v>0</v>
@@ -8401,11 +8402,11 @@
         <v>2</v>
       </c>
       <c r="J18">
-        <f>AVERAGE(B$6:B$8)-MIN(J3:J12)</f>
-        <v>0.36433333333333318</v>
+        <f>AVERAGE(B$6:B$8)-J$11</f>
+        <v>0.24766666666666648</v>
       </c>
       <c r="K18">
-        <f t="shared" ref="K18:O18" si="11">AVERAGE(C$6:C$8)-MIN(K3:K12)</f>
+        <f t="shared" ref="K18:O18" si="11">AVERAGE(C$6:C$8)-K$11</f>
         <v>0.24399999999999977</v>
       </c>
       <c r="L18">
@@ -8414,15 +8415,15 @@
       </c>
       <c r="M18">
         <f t="shared" si="11"/>
-        <v>0.16300000000000026</v>
+        <v>-9.733333333333416E-2</v>
       </c>
       <c r="N18">
         <f t="shared" si="11"/>
-        <v>0.13733333333333064</v>
+        <v>-0.27300000000000324</v>
       </c>
       <c r="O18">
         <f t="shared" si="11"/>
-        <v>9.5999999999999974E-2</v>
+        <v>4.1666666666666741E-2</v>
       </c>
       <c r="R18" t="str">
         <v>Spark</v>
@@ -8431,34 +8432,34 @@
         <v>spark real</v>
       </c>
       <c r="T18">
-        <v>0.41266666666666829</v>
+        <v>0.15233333333333388</v>
       </c>
       <c r="U18">
-        <v>0.16300000000000026</v>
+        <v>-9.733333333333416E-2</v>
       </c>
       <c r="V18">
-        <v>9.4333333333334046E-2</v>
+        <v>-0.16600000000000037</v>
       </c>
       <c r="W18">
-        <v>0.30000000000000071</v>
+        <v>3.9666666666666295E-2</v>
       </c>
       <c r="X18">
-        <v>0.18866666666666809</v>
+        <v>-7.1666666666666323E-2</v>
       </c>
       <c r="Y18">
-        <v>0.30400000000000116</v>
+        <v>4.3666666666666742E-2</v>
       </c>
       <c r="Z18">
-        <v>0.14000000000000057</v>
+        <v>-0.12033333333333385</v>
       </c>
       <c r="AA18">
+        <v>-0.26033333333333442</v>
+      </c>
+      <c r="AB18">
         <v>0</v>
       </c>
-      <c r="AB18">
-        <v>0.26033333333333442</v>
-      </c>
       <c r="AC18">
-        <v>0.97500000000000053</v>
+        <v>0.71466666666666612</v>
       </c>
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.25">
@@ -8487,11 +8488,11 @@
         <v>3</v>
       </c>
       <c r="J19">
-        <f>AVERAGE(B$9:B$11)-MIN(J3:J12)</f>
-        <v>0.42933333333333357</v>
+        <f>AVERAGE(B$9:B$11)-J$11</f>
+        <v>0.31266666666666687</v>
       </c>
       <c r="K19">
-        <f t="shared" ref="K19:O19" si="12">AVERAGE(C$9:C$11)-MIN(K3:K12)</f>
+        <f t="shared" ref="K19:O19" si="12">AVERAGE(C$9:C$11)-K$11</f>
         <v>0.82599999999999962</v>
       </c>
       <c r="L19">
@@ -8500,15 +8501,15 @@
       </c>
       <c r="M19">
         <f t="shared" si="12"/>
-        <v>9.4333333333334046E-2</v>
+        <v>-0.16600000000000037</v>
       </c>
       <c r="N19">
         <f t="shared" si="12"/>
-        <v>0.18066666666666364</v>
+        <v>-0.22966666666667024</v>
       </c>
       <c r="O19">
         <f t="shared" si="12"/>
-        <v>2.9333333333333211E-2</v>
+        <v>-2.5000000000000022E-2</v>
       </c>
       <c r="R19">
         <v>0</v>
@@ -8517,34 +8518,34 @@
         <v>spark user</v>
       </c>
       <c r="T19">
-        <v>0.93666666666666387</v>
+        <v>0.52633333333332999</v>
       </c>
       <c r="U19">
-        <v>0.13733333333333064</v>
+        <v>-0.27300000000000324</v>
       </c>
       <c r="V19">
-        <v>0.18066666666666364</v>
+        <v>-0.22966666666667024</v>
       </c>
       <c r="W19">
-        <v>1.2456666666666649</v>
+        <v>0.83533333333333104</v>
       </c>
       <c r="X19">
+        <v>-0.41033333333333388</v>
+      </c>
+      <c r="Y19">
+        <v>0.46733333333333249</v>
+      </c>
+      <c r="Z19">
+        <v>0.16866666666666319</v>
+      </c>
+      <c r="AA19">
+        <v>-0.16766666666666907</v>
+      </c>
+      <c r="AB19">
         <v>0</v>
       </c>
-      <c r="Y19">
-        <v>0.87766666666666637</v>
-      </c>
-      <c r="Z19">
-        <v>0.57899999999999707</v>
-      </c>
-      <c r="AA19">
-        <v>0.24266666666666481</v>
-      </c>
-      <c r="AB19">
-        <v>0.41033333333333388</v>
-      </c>
       <c r="AC19">
-        <v>1.4706666666666628</v>
+        <v>1.0603333333333289</v>
       </c>
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.25">
@@ -8573,11 +8574,11 @@
         <v>4</v>
       </c>
       <c r="J20">
-        <f>AVERAGE(B$12:B$14)-MIN(J3:J12)</f>
-        <v>0.71400000000000086</v>
+        <f>AVERAGE(B$12:B$14)-J$11</f>
+        <v>0.59733333333333416</v>
       </c>
       <c r="K20">
-        <f t="shared" ref="K20:O20" si="13">AVERAGE(C$12:C$14)-MIN(K3:K12)</f>
+        <f t="shared" ref="K20:O20" si="13">AVERAGE(C$12:C$14)-K$11</f>
         <v>0.87799999999999923</v>
       </c>
       <c r="L20">
@@ -8586,15 +8587,15 @@
       </c>
       <c r="M20">
         <f t="shared" si="13"/>
-        <v>0.30000000000000071</v>
+        <v>3.9666666666666295E-2</v>
       </c>
       <c r="N20">
         <f t="shared" si="13"/>
-        <v>1.2456666666666649</v>
+        <v>0.83533333333333104</v>
       </c>
       <c r="O20">
         <f t="shared" si="13"/>
-        <v>2.8333333333333321E-2</v>
+        <v>-2.5999999999999912E-2</v>
       </c>
       <c r="R20">
         <v>0</v>
@@ -8603,34 +8604,34 @@
         <v>spark sys</v>
       </c>
       <c r="T20">
-        <v>4.3333333333333335E-2</v>
+        <v>-1.0999999999999899E-2</v>
       </c>
       <c r="U20">
-        <v>9.5999999999999974E-2</v>
+        <v>4.1666666666666741E-2</v>
       </c>
       <c r="V20">
-        <v>2.9333333333333211E-2</v>
+        <v>-2.5000000000000022E-2</v>
       </c>
       <c r="W20">
-        <v>2.8333333333333321E-2</v>
+        <v>-2.5999999999999912E-2</v>
       </c>
       <c r="X20">
-        <v>1.3999999999999901E-2</v>
+        <v>-4.0333333333333332E-2</v>
       </c>
       <c r="Y20">
-        <v>5.1333333333333342E-2</v>
+        <v>-2.9999999999998916E-3</v>
       </c>
       <c r="Z20">
-        <v>4.5666666666666633E-2</v>
+        <v>-8.6666666666666003E-3</v>
       </c>
       <c r="AA20">
+        <v>-5.4333333333333234E-2</v>
+      </c>
+      <c r="AB20">
         <v>0</v>
       </c>
-      <c r="AB20">
-        <v>5.4333333333333234E-2</v>
-      </c>
       <c r="AC20">
-        <v>4.3666666666666631E-2</v>
+        <v>-1.0666666666666602E-2</v>
       </c>
     </row>
     <row r="21" spans="1:29" x14ac:dyDescent="0.25">
@@ -8659,11 +8660,11 @@
         <v>5</v>
       </c>
       <c r="J21">
-        <f>AVERAGE(B$15:B$17)-MIN(J3:J12)</f>
-        <v>8.1333333333333258E-2</v>
+        <f>AVERAGE(B$15:B$17)-J$11</f>
+        <v>-3.5333333333333439E-2</v>
       </c>
       <c r="K21">
-        <f t="shared" ref="K21:O21" si="14">AVERAGE(C$15:C$17)-MIN(K3:K12)</f>
+        <f t="shared" ref="K21:O21" si="14">AVERAGE(C$15:C$17)-K$11</f>
         <v>0.69866666666666699</v>
       </c>
       <c r="L21">
@@ -8672,15 +8673,15 @@
       </c>
       <c r="M21">
         <f t="shared" si="14"/>
-        <v>0.18866666666666809</v>
+        <v>-7.1666666666666323E-2</v>
       </c>
       <c r="N21">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>-0.41033333333333388</v>
       </c>
       <c r="O21">
         <f t="shared" si="14"/>
-        <v>1.3999999999999901E-2</v>
+        <v>-4.0333333333333332E-2</v>
       </c>
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.25">
@@ -8709,11 +8710,11 @@
         <v>6</v>
       </c>
       <c r="J22">
-        <f>AVERAGE(B$18:B$20)-MIN(J3:J12)</f>
-        <v>0.10133333333333372</v>
+        <f>AVERAGE(B$18:B$20)-J$11</f>
+        <v>-1.5333333333332977E-2</v>
       </c>
       <c r="K22">
-        <f t="shared" ref="K22:O22" si="15">AVERAGE(C$18:C$20)-MIN(K3:K12)</f>
+        <f t="shared" ref="K22:O22" si="15">AVERAGE(C$18:C$20)-K$11</f>
         <v>0.40200000000000014</v>
       </c>
       <c r="L22">
@@ -8722,15 +8723,15 @@
       </c>
       <c r="M22">
         <f t="shared" si="15"/>
-        <v>0.30400000000000116</v>
+        <v>4.3666666666666742E-2</v>
       </c>
       <c r="N22">
         <f t="shared" si="15"/>
-        <v>0.87766666666666637</v>
+        <v>0.46733333333333249</v>
       </c>
       <c r="O22">
         <f t="shared" si="15"/>
-        <v>5.1333333333333342E-2</v>
+        <v>-2.9999999999998916E-3</v>
       </c>
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.25">
@@ -8759,11 +8760,11 @@
         <v>7</v>
       </c>
       <c r="J23">
-        <f>AVERAGE(B$21:B$23)-MIN(J3:J12)</f>
-        <v>0.3660000000000001</v>
+        <f>AVERAGE(B$21:B$23)-J$11</f>
+        <v>0.24933333333333341</v>
       </c>
       <c r="K23">
-        <f t="shared" ref="K23:O23" si="16">AVERAGE(C$21:C$23)-MIN(K3:K12)</f>
+        <f t="shared" ref="K23:O23" si="16">AVERAGE(C$21:C$23)-K$11</f>
         <v>0.18933333333333291</v>
       </c>
       <c r="L23">
@@ -8772,15 +8773,15 @@
       </c>
       <c r="M23">
         <f t="shared" si="16"/>
-        <v>0.14000000000000057</v>
+        <v>-0.12033333333333385</v>
       </c>
       <c r="N23">
         <f t="shared" si="16"/>
-        <v>0.57899999999999707</v>
+        <v>0.16866666666666319</v>
       </c>
       <c r="O23">
         <f t="shared" si="16"/>
-        <v>4.5666666666666633E-2</v>
+        <v>-8.6666666666666003E-3</v>
       </c>
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.25">
@@ -8809,11 +8810,11 @@
         <v>8</v>
       </c>
       <c r="J24">
-        <f>AVERAGE(B$24:B$26)-MIN(J3:J12)</f>
-        <v>0</v>
+        <f>AVERAGE(B$24:B$26)-J$11</f>
+        <v>-0.1166666666666667</v>
       </c>
       <c r="K24">
-        <f t="shared" ref="K24:O24" si="17">AVERAGE(C$24:C$26)-MIN(K3:K12)</f>
+        <f t="shared" ref="K24:O24" si="17">AVERAGE(C$24:C$26)-K$11</f>
         <v>9.3666666666666565E-2</v>
       </c>
       <c r="L24">
@@ -8822,15 +8823,15 @@
       </c>
       <c r="M24">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>-0.26033333333333442</v>
       </c>
       <c r="N24">
         <f t="shared" si="17"/>
-        <v>0.24266666666666481</v>
+        <v>-0.16766666666666907</v>
       </c>
       <c r="O24">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>-5.4333333333333234E-2</v>
       </c>
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.25">
@@ -8859,11 +8860,11 @@
         <v>9</v>
       </c>
       <c r="J25">
-        <f>AVERAGE(B$27:B$29)-MIN(J3:J12)</f>
-        <v>0.1166666666666667</v>
+        <f>AVERAGE(B$27:B$29)-J$11</f>
+        <v>0</v>
       </c>
       <c r="K25">
-        <f t="shared" ref="K25:O25" si="18">AVERAGE(C$27:C$29)-MIN(K3:K12)</f>
+        <f t="shared" ref="K25:O25" si="18">AVERAGE(C$27:C$29)-K$11</f>
         <v>0</v>
       </c>
       <c r="L25">
@@ -8872,15 +8873,15 @@
       </c>
       <c r="M25">
         <f t="shared" si="18"/>
-        <v>0.26033333333333442</v>
+        <v>0</v>
       </c>
       <c r="N25">
         <f t="shared" si="18"/>
-        <v>0.41033333333333388</v>
+        <v>0</v>
       </c>
       <c r="O25">
         <f t="shared" si="18"/>
-        <v>5.4333333333333234E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.25">
@@ -8909,11 +8910,11 @@
         <v>10</v>
       </c>
       <c r="J26">
-        <f>AVERAGE(B$30:B$32)-MIN(J3:J12)</f>
-        <v>1.0623333333333336</v>
+        <f>AVERAGE(B$30:B$32)-J$11</f>
+        <v>0.94566666666666688</v>
       </c>
       <c r="K26">
-        <f t="shared" ref="K26:O26" si="19">AVERAGE(C$30:C$32)-MIN(K3:K12)</f>
+        <f t="shared" ref="K26:O26" si="19">AVERAGE(C$30:C$32)-K$11</f>
         <v>2.4133333333333349</v>
       </c>
       <c r="L26">
@@ -8922,15 +8923,15 @@
       </c>
       <c r="M26">
         <f t="shared" si="19"/>
-        <v>0.97500000000000053</v>
+        <v>0.71466666666666612</v>
       </c>
       <c r="N26">
         <f t="shared" si="19"/>
-        <v>1.4706666666666628</v>
+        <v>1.0603333333333289</v>
       </c>
       <c r="O26">
         <f t="shared" si="19"/>
-        <v>4.3666666666666631E-2</v>
+        <v>-1.0666666666666602E-2</v>
       </c>
     </row>
     <row r="27" spans="1:29" x14ac:dyDescent="0.25">

</xml_diff>